<commit_message>
added distance matrix based on adjacency in an excel csv file, among other godly things
</commit_message>
<xml_diff>
--- a/resources/adj_matrix.xlsx
+++ b/resources/adj_matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="60" windowWidth="11460" windowHeight="5568" tabRatio="209" activeTab="1"/>
+    <workbookView xWindow="288" yWindow="120" windowWidth="11460" windowHeight="5508" tabRatio="209" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Numbered Map" sheetId="1" r:id="rId1"/>
@@ -552,7 +552,7 @@
   <dimension ref="A1:CJ82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6189,9 +6189,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomLeft" activeCell="BH56" sqref="BH56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>